<commit_message>
Some fixes to Excel and N.E.
</commit_message>
<xml_diff>
--- a/files/Dice Poker Riddler vF.xlsx
+++ b/files/Dice Poker Riddler vF.xlsx
@@ -194,9 +194,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -341,6 +343,24 @@
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -356,26 +376,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="64">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -407,6 +409,7 @@
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -437,9 +440,10 @@
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
     <dxf>
       <border>
         <left style="thin">
@@ -469,6 +473,38 @@
         </top>
         <bottom style="thin">
           <color rgb="FF9C0006"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
         </bottom>
       </border>
     </dxf>
@@ -833,7 +869,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -849,25 +887,25 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="32" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="35" t="s">
+      <c r="M3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
     </row>
     <row r="4" spans="1:15">
       <c r="B4" s="25"/>
@@ -895,18 +933,18 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M4" s="38" t="s">
+      <c r="M4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="38" t="s">
+      <c r="N4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="38" t="s">
+      <c r="O4" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="28">
@@ -939,7 +977,7 @@
       <c r="M5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="39">
+      <c r="N5" s="31">
         <v>3</v>
       </c>
       <c r="O5" s="17">
@@ -948,7 +986,7 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="B6" s="31"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="27">
         <f>C5-1</f>
         <v>5</v>
@@ -980,7 +1018,7 @@
       <c r="M6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="40">
+      <c r="N6" s="32">
         <v>4</v>
       </c>
       <c r="O6" s="18">
@@ -989,7 +1027,7 @@
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="B7" s="31"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="27">
         <f t="shared" ref="C7:C10" si="2">C6-1</f>
         <v>4</v>
@@ -1020,7 +1058,7 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="B8" s="31"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="27">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -1051,7 +1089,7 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="B9" s="31"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="27">
         <f t="shared" si="2"/>
         <v>2</v>
@@ -1082,7 +1120,7 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="B10" s="31"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="27">
         <f t="shared" si="2"/>
         <v>1</v>
@@ -1113,27 +1151,27 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="32" t="s">
+      <c r="C12" s="35"/>
+      <c r="D12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="32" t="s">
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="31"/>
-      <c r="M12" s="35" t="s">
+      <c r="K12" s="37"/>
+      <c r="M12" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
     </row>
     <row r="13" spans="1:15">
       <c r="B13" s="25"/>
@@ -1170,7 +1208,7 @@
       <c r="K13" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="M13" s="38" t="s">
+      <c r="M13" s="30" t="s">
         <v>9</v>
       </c>
       <c r="N13" s="27" t="s">
@@ -1181,7 +1219,7 @@
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="39" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="28">
@@ -1207,7 +1245,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="8">
-        <f t="array" ref="J14">MIN(IF(D14:I14=K14, D$13:I$13, 7))</f>
+        <f t="array" ref="J14">MAX(IF(D14:I14=K14, D$13:I$13, -1))</f>
         <v>6</v>
       </c>
       <c r="K14" s="11">
@@ -1227,7 +1265,7 @@
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="B15" s="34"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="27">
         <f>C14-1</f>
         <v>5</v>
@@ -1251,8 +1289,8 @@
         <v>0</v>
       </c>
       <c r="J15" s="9">
-        <f t="array" ref="J15">MIN(IF(D15:I15=K15, D$13:I$13, 7))</f>
-        <v>5</v>
+        <f t="array" ref="J15">MAX(IF(D15:I15=K15, D$13:I$13, -1))</f>
+        <v>6</v>
       </c>
       <c r="K15" s="13">
         <f t="shared" si="4"/>
@@ -1264,7 +1302,7 @@
       </c>
       <c r="N15" s="24">
         <f>INDEX(J14:J19,7-$N$14)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O15" s="6">
         <f>INDEX(K14:K19,7-$N$14)</f>
@@ -1272,7 +1310,7 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="B16" s="34"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="27">
         <f t="shared" ref="C16:C19" si="5">C15-1</f>
         <v>4</v>
@@ -1296,7 +1334,7 @@
         <v>-5.5555555555555552E-2</v>
       </c>
       <c r="J16" s="9">
-        <f t="array" ref="J16">MIN(IF(D16:I16=K16, D$13:I$13, 7))</f>
+        <f t="array" ref="J16">MAX(IF(D16:I16=K16, D$13:I$13, -1))</f>
         <v>5</v>
       </c>
       <c r="K16" s="13">
@@ -1307,7 +1345,7 @@
       <c r="M16" s="4"/>
     </row>
     <row r="17" spans="2:16">
-      <c r="B17" s="34"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="27">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -1331,7 +1369,7 @@
         <v>-0.16666666666666666</v>
       </c>
       <c r="J17" s="9">
-        <f t="array" ref="J17">MIN(IF(D17:I17=K17, D$13:I$13, 7))</f>
+        <f t="array" ref="J17">MAX(IF(D17:I17=K17, D$13:I$13, -1))</f>
         <v>4</v>
       </c>
       <c r="K17" s="13">
@@ -1342,7 +1380,7 @@
       <c r="M17" s="4"/>
     </row>
     <row r="18" spans="2:16">
-      <c r="B18" s="34"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="27">
         <f t="shared" si="5"/>
         <v>2</v>
@@ -1366,7 +1404,7 @@
         <v>-0.33333333333333331</v>
       </c>
       <c r="J18" s="9">
-        <f t="array" ref="J18">MIN(IF(D18:I18=K18, D$13:I$13, 7))</f>
+        <f t="array" ref="J18">MAX(IF(D18:I18=K18, D$13:I$13, -1))</f>
         <v>3</v>
       </c>
       <c r="K18" s="13">
@@ -1378,7 +1416,7 @@
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="2:16">
-      <c r="B19" s="34"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="27">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -1402,8 +1440,8 @@
         <v>-0.55555555555555558</v>
       </c>
       <c r="J19" s="9">
-        <f t="array" ref="J19">MIN(IF(D19:I19=K19, D$13:I$13, 7))</f>
-        <v>2</v>
+        <f t="array" ref="J19">MAX(IF(D19:I19=K19, D$13:I$13, -1))</f>
+        <v>3</v>
       </c>
       <c r="K19" s="13">
         <f t="shared" si="4"/>
@@ -1427,6 +1465,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="J12:K12"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="M12:O12"/>
     <mergeCell ref="B12:C12"/>
@@ -1434,15 +1474,13 @@
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="D12:I12"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="J12:K12"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:I19">
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
-      <formula>AND(D14=$O$15, D14=$K14)</formula>
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+      <formula>AND(D14=$O$15, D$13=$J14)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>(D14=$K14)</formula>
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>(D$13=$J14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:I10">

</xml_diff>